<commit_message>
Image creation and text
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KnossosTombs.xlsx
+++ b/analysis/data/raw_data/KnossosTombs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcpol\domproject\analysis\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CC1E9BF-9AC1-4EC7-9814-941EAAAE6836}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{86D66AE0-D2C3-46FA-B5A9-250B7688FD0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{C5AF37E9-EE35-4170-9AC2-549D3F969642}"/>
   </bookViews>
@@ -1472,7 +1472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708C975D-686F-4ADC-B3DB-5AE93DD73972}">
   <dimension ref="A1:GX155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -59033,7 +59035,7 @@
         <v>137</v>
       </c>
       <c r="C100" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="D100" t="s">
         <v>62</v>
@@ -65927,7 +65929,7 @@
         <v>160</v>
       </c>
       <c r="C112" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="D112" t="s">
         <v>62</v>
@@ -66508,7 +66510,7 @@
         <v>160</v>
       </c>
       <c r="C113" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="D113" t="s">
         <v>62</v>
@@ -67083,7 +67085,7 @@
         <v>160</v>
       </c>
       <c r="C114" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="D114" t="s">
         <v>62</v>
@@ -67661,7 +67663,7 @@
         <v>160</v>
       </c>
       <c r="C115" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="D115" t="s">
         <v>62</v>
@@ -68239,7 +68241,7 @@
         <v>160</v>
       </c>
       <c r="C116" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="D116" t="s">
         <v>62</v>
@@ -68790,7 +68792,7 @@
         <v>160</v>
       </c>
       <c r="C117" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="D117" t="s">
         <v>62</v>
@@ -69368,7 +69370,7 @@
         <v>160</v>
       </c>
       <c r="C118" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="D118" t="s">
         <v>62</v>
@@ -69937,7 +69939,7 @@
         <v>160</v>
       </c>
       <c r="C119" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="D119" t="s">
         <v>62</v>
@@ -70509,7 +70511,7 @@
         <v>160</v>
       </c>
       <c r="C120" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="D120" t="s">
         <v>62</v>
@@ -71084,7 +71086,7 @@
         <v>160</v>
       </c>
       <c r="C121" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="D121" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Writing and image importing
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KnossosTombs.xlsx
+++ b/analysis/data/raw_data/KnossosTombs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcpol\domproject\analysis\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3550C2-50AA-4189-86DC-DDAE30D84304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8572F961-E5AC-4BB3-A3A3-7CF6569D30F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="365">
   <si>
     <t>tomb_type_condensed</t>
   </si>
@@ -1113,6 +1113,9 @@
   <si>
     <t>KNC</t>
   </si>
+  <si>
+    <t>polychrome_pithoi</t>
+  </si>
 </sst>
 </file>
 
@@ -1952,15 +1955,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IW155"/>
+  <dimension ref="A1:IX155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C136" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="IB1" workbookViewId="0">
+      <selection activeCell="IX4" sqref="IX4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>353</v>
       </c>
@@ -2732,8 +2735,11 @@
       <c r="IW1" t="s">
         <v>196</v>
       </c>
+      <c r="IX1" t="s">
+        <v>364</v>
+      </c>
     </row>
-    <row r="2" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3454,8 +3460,11 @@
       <c r="IW2">
         <v>0</v>
       </c>
+      <c r="IX2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4188,8 +4197,11 @@
       <c r="IW3">
         <v>0</v>
       </c>
+      <c r="IX3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
@@ -4910,8 +4922,11 @@
       <c r="IW4">
         <v>0</v>
       </c>
+      <c r="IX4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>9</v>
       </c>
@@ -5605,8 +5620,11 @@
       <c r="IW5">
         <v>0</v>
       </c>
+      <c r="IX5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>13</v>
       </c>
@@ -6354,8 +6372,11 @@
       <c r="IW6">
         <v>0</v>
       </c>
+      <c r="IX6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>14</v>
       </c>
@@ -7094,8 +7115,11 @@
       <c r="IW7">
         <v>0</v>
       </c>
+      <c r="IX7">
+        <v>3</v>
+      </c>
     </row>
-    <row r="8" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>16</v>
       </c>
@@ -7828,8 +7852,11 @@
       <c r="IW8">
         <v>0</v>
       </c>
+      <c r="IX8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>18</v>
       </c>
@@ -8574,8 +8601,11 @@
       <c r="IW9">
         <v>0</v>
       </c>
+      <c r="IX9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>19</v>
       </c>
@@ -9320,8 +9350,11 @@
       <c r="IW10">
         <v>0</v>
       </c>
+      <c r="IX10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>24</v>
       </c>
@@ -10063,8 +10096,11 @@
       <c r="IW11">
         <v>0</v>
       </c>
+      <c r="IX11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>25</v>
       </c>
@@ -10806,8 +10842,11 @@
       <c r="IW12">
         <v>0</v>
       </c>
+      <c r="IX12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>26</v>
       </c>
@@ -11546,8 +11585,11 @@
       <c r="IW13">
         <v>0</v>
       </c>
+      <c r="IX13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>28</v>
       </c>
@@ -12292,8 +12334,11 @@
       <c r="IW14">
         <v>0</v>
       </c>
+      <c r="IX14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>30</v>
       </c>
@@ -13032,8 +13077,11 @@
       <c r="IW15">
         <v>0</v>
       </c>
+      <c r="IX15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>31</v>
       </c>
@@ -13760,8 +13808,11 @@
       <c r="IW16">
         <v>0</v>
       </c>
+      <c r="IX16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>34</v>
       </c>
@@ -14497,8 +14548,11 @@
       <c r="IW17">
         <v>0</v>
       </c>
+      <c r="IX17">
+        <v>3</v>
+      </c>
     </row>
-    <row r="18" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>40</v>
       </c>
@@ -15243,8 +15297,11 @@
       <c r="IW18">
         <v>0</v>
       </c>
+      <c r="IX18">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>44</v>
       </c>
@@ -15953,8 +16010,11 @@
       <c r="IW19">
         <v>0</v>
       </c>
+      <c r="IX19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>45</v>
       </c>
@@ -16696,8 +16756,11 @@
       <c r="IW20">
         <v>0</v>
       </c>
+      <c r="IX20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>48</v>
       </c>
@@ -17445,8 +17508,11 @@
       <c r="IW21">
         <v>0</v>
       </c>
+      <c r="IX21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>55</v>
       </c>
@@ -18179,8 +18245,11 @@
       <c r="IW22">
         <v>0</v>
       </c>
+      <c r="IX22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>56</v>
       </c>
@@ -18925,8 +18994,11 @@
       <c r="IW23">
         <v>0</v>
       </c>
+      <c r="IX23">
+        <v>2</v>
+      </c>
     </row>
-    <row r="24" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>57</v>
       </c>
@@ -19659,8 +19731,11 @@
       <c r="IW24">
         <v>0</v>
       </c>
+      <c r="IX24">
+        <v>2</v>
+      </c>
     </row>
-    <row r="25" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>59</v>
       </c>
@@ -20390,8 +20465,11 @@
       <c r="IW25">
         <v>0</v>
       </c>
+      <c r="IX25">
+        <v>2</v>
+      </c>
     </row>
-    <row r="26" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>60</v>
       </c>
@@ -21151,8 +21229,11 @@
       <c r="IW26">
         <v>0</v>
       </c>
+      <c r="IX26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>61</v>
       </c>
@@ -21906,8 +21987,11 @@
       <c r="IW27">
         <v>0</v>
       </c>
+      <c r="IX27">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>63</v>
       </c>
@@ -22634,8 +22718,11 @@
       <c r="IW28">
         <v>0</v>
       </c>
+      <c r="IX28">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>69</v>
       </c>
@@ -23350,8 +23437,11 @@
       <c r="IW29">
         <v>0</v>
       </c>
+      <c r="IX29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>75</v>
       </c>
@@ -24102,8 +24192,11 @@
       <c r="IW30">
         <v>0</v>
       </c>
+      <c r="IX30">
+        <v>14</v>
+      </c>
     </row>
-    <row r="31" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>76</v>
       </c>
@@ -24833,8 +24926,11 @@
       <c r="IW31">
         <v>0</v>
       </c>
+      <c r="IX31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>78</v>
       </c>
@@ -25552,8 +25648,11 @@
       <c r="IW32">
         <v>0</v>
       </c>
+      <c r="IX32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>79</v>
       </c>
@@ -26283,8 +26382,11 @@
       <c r="IW33">
         <v>0</v>
       </c>
+      <c r="IX33">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>80</v>
       </c>
@@ -27011,8 +27113,11 @@
       <c r="IW34">
         <v>0</v>
       </c>
+      <c r="IX34">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>82</v>
       </c>
@@ -27748,8 +27853,11 @@
       <c r="IW35">
         <v>0</v>
       </c>
+      <c r="IX35">
+        <v>3</v>
+      </c>
     </row>
-    <row r="36" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>85</v>
       </c>
@@ -28473,8 +28581,11 @@
       <c r="IW36">
         <v>0</v>
       </c>
+      <c r="IX36">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>86</v>
       </c>
@@ -29177,8 +29288,11 @@
       <c r="IW37">
         <v>0</v>
       </c>
+      <c r="IX37">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>98</v>
       </c>
@@ -29920,8 +30034,11 @@
       <c r="IW38">
         <v>0</v>
       </c>
+      <c r="IX38">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>100</v>
       </c>
@@ -30672,8 +30789,11 @@
       <c r="IW39">
         <v>0</v>
       </c>
+      <c r="IX39">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>103</v>
       </c>
@@ -31400,8 +31520,11 @@
       <c r="IW40">
         <v>0</v>
       </c>
+      <c r="IX40">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>104</v>
       </c>
@@ -32137,8 +32260,11 @@
       <c r="IW41">
         <v>0</v>
       </c>
+      <c r="IX41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>105</v>
       </c>
@@ -32853,8 +32979,11 @@
       <c r="IW42">
         <v>0</v>
       </c>
+      <c r="IX42">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>106</v>
       </c>
@@ -33605,8 +33734,11 @@
       <c r="IW43">
         <v>0</v>
       </c>
+      <c r="IX43">
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>107</v>
       </c>
@@ -34354,8 +34486,11 @@
       <c r="IW44">
         <v>0</v>
       </c>
+      <c r="IX44">
+        <v>4</v>
+      </c>
     </row>
-    <row r="45" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>111</v>
       </c>
@@ -35070,8 +35205,11 @@
       <c r="IW45">
         <v>0</v>
       </c>
+      <c r="IX45">
+        <v>1</v>
+      </c>
     </row>
-    <row r="46" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>112</v>
       </c>
@@ -35807,8 +35945,11 @@
       <c r="IW46">
         <v>0</v>
       </c>
+      <c r="IX46">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>113</v>
       </c>
@@ -36526,8 +36667,11 @@
       <c r="IW47">
         <v>0</v>
       </c>
+      <c r="IX47">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>121</v>
       </c>
@@ -37257,8 +37401,11 @@
       <c r="IW48">
         <v>0</v>
       </c>
+      <c r="IX48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>123</v>
       </c>
@@ -37991,8 +38138,11 @@
       <c r="IW49">
         <v>0</v>
       </c>
+      <c r="IX49">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>125</v>
       </c>
@@ -38725,8 +38875,11 @@
       <c r="IW50">
         <v>0</v>
       </c>
+      <c r="IX50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>126</v>
       </c>
@@ -39444,8 +39597,11 @@
       <c r="IW51">
         <v>0</v>
       </c>
+      <c r="IX51">
+        <v>1</v>
+      </c>
     </row>
-    <row r="52" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>129</v>
       </c>
@@ -40184,8 +40340,11 @@
       <c r="IW52">
         <v>0</v>
       </c>
+      <c r="IX52">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>132</v>
       </c>
@@ -40936,8 +41095,11 @@
       <c r="IW53">
         <v>0</v>
       </c>
+      <c r="IX53">
+        <v>2</v>
+      </c>
     </row>
-    <row r="54" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>134</v>
       </c>
@@ -41676,8 +41838,11 @@
       <c r="IW54">
         <v>0</v>
       </c>
+      <c r="IX54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>135</v>
       </c>
@@ -42401,8 +42566,11 @@
       <c r="IW55">
         <v>0</v>
       </c>
+      <c r="IX55">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>138</v>
       </c>
@@ -43132,8 +43300,11 @@
       <c r="IW56">
         <v>0</v>
       </c>
+      <c r="IX56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>146</v>
       </c>
@@ -43866,8 +44037,11 @@
       <c r="IW57">
         <v>0</v>
       </c>
+      <c r="IX57">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>147</v>
       </c>
@@ -44597,8 +44771,11 @@
       <c r="IW58">
         <v>0</v>
       </c>
+      <c r="IX58">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>149</v>
       </c>
@@ -45322,8 +45499,11 @@
       <c r="IW59">
         <v>0</v>
       </c>
+      <c r="IX59">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>152</v>
       </c>
@@ -46059,8 +46239,11 @@
       <c r="IW60">
         <v>0</v>
       </c>
+      <c r="IX60">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>153</v>
       </c>
@@ -46784,8 +46967,11 @@
       <c r="IW61">
         <v>0</v>
       </c>
+      <c r="IX61">
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>159</v>
       </c>
@@ -47503,8 +47689,11 @@
       <c r="IW62">
         <v>0</v>
       </c>
+      <c r="IX62">
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>160</v>
       </c>
@@ -48228,8 +48417,11 @@
       <c r="IW63">
         <v>0</v>
       </c>
+      <c r="IX63">
+        <v>0</v>
+      </c>
     </row>
-    <row r="64" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>163</v>
       </c>
@@ -48956,8 +49148,11 @@
       <c r="IW64">
         <v>0</v>
       </c>
+      <c r="IX64">
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>168</v>
       </c>
@@ -49684,8 +49879,11 @@
       <c r="IW65">
         <v>0</v>
       </c>
+      <c r="IX65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>175</v>
       </c>
@@ -50439,8 +50637,11 @@
       <c r="IW66">
         <v>0</v>
       </c>
+      <c r="IX66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>176</v>
       </c>
@@ -51146,8 +51347,11 @@
       <c r="IW67">
         <v>0</v>
       </c>
+      <c r="IX67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>182</v>
       </c>
@@ -51874,8 +52078,11 @@
       <c r="IW68">
         <v>0</v>
       </c>
+      <c r="IX68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>186</v>
       </c>
@@ -52599,8 +52806,11 @@
       <c r="IW69">
         <v>0</v>
       </c>
+      <c r="IX69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>200</v>
       </c>
@@ -53327,8 +53537,11 @@
       <c r="IW70">
         <v>0</v>
       </c>
+      <c r="IX70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>201</v>
       </c>
@@ -54055,8 +54268,11 @@
       <c r="IW71">
         <v>0</v>
       </c>
+      <c r="IX71">
+        <v>0</v>
+      </c>
     </row>
-    <row r="72" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>202</v>
       </c>
@@ -54780,8 +54996,11 @@
       <c r="IW72">
         <v>0</v>
       </c>
+      <c r="IX72">
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>207</v>
       </c>
@@ -55523,8 +55742,11 @@
       <c r="IW73">
         <v>0</v>
       </c>
+      <c r="IX73">
+        <v>0</v>
+      </c>
     </row>
-    <row r="74" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>208</v>
       </c>
@@ -56251,8 +56473,11 @@
       <c r="IW74">
         <v>0</v>
       </c>
+      <c r="IX74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="75" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>218</v>
       </c>
@@ -57003,8 +57228,11 @@
       <c r="IW75">
         <v>0</v>
       </c>
+      <c r="IX75">
+        <v>0</v>
+      </c>
     </row>
-    <row r="76" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>219</v>
       </c>
@@ -57767,8 +57995,11 @@
       <c r="IW76">
         <v>0</v>
       </c>
+      <c r="IX76">
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>221</v>
       </c>
@@ -58480,8 +58711,11 @@
       <c r="IW77">
         <v>0</v>
       </c>
+      <c r="IX77">
+        <v>0</v>
+      </c>
     </row>
-    <row r="78" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>222</v>
       </c>
@@ -59205,8 +59439,11 @@
       <c r="IW78">
         <v>0</v>
       </c>
+      <c r="IX78">
+        <v>0</v>
+      </c>
     </row>
-    <row r="79" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>229</v>
       </c>
@@ -59954,8 +60191,11 @@
       <c r="IW79">
         <v>0</v>
       </c>
+      <c r="IX79">
+        <v>1</v>
+      </c>
     </row>
-    <row r="80" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>242</v>
       </c>
@@ -60682,8 +60922,11 @@
       <c r="IW80">
         <v>0</v>
       </c>
+      <c r="IX80">
+        <v>0</v>
+      </c>
     </row>
-    <row r="81" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>247</v>
       </c>
@@ -61377,8 +61620,11 @@
       <c r="IW81">
         <v>0</v>
       </c>
+      <c r="IX81">
+        <v>0</v>
+      </c>
     </row>
-    <row r="82" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>280</v>
       </c>
@@ -62102,8 +62348,11 @@
       <c r="IW82">
         <v>0</v>
       </c>
+      <c r="IX82">
+        <v>0</v>
+      </c>
     </row>
-    <row r="83" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>282</v>
       </c>
@@ -62830,8 +63079,11 @@
       <c r="IW83">
         <v>0</v>
       </c>
+      <c r="IX83">
+        <v>0</v>
+      </c>
     </row>
-    <row r="84" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>283</v>
       </c>
@@ -63585,8 +63837,11 @@
       <c r="IW84">
         <v>0</v>
       </c>
+      <c r="IX84">
+        <v>0</v>
+      </c>
     </row>
-    <row r="85" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>285</v>
       </c>
@@ -64349,8 +64604,11 @@
       <c r="IW85">
         <v>0</v>
       </c>
+      <c r="IX85">
+        <v>8</v>
+      </c>
     </row>
-    <row r="86" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>286</v>
       </c>
@@ -65086,8 +65344,11 @@
       <c r="IW86">
         <v>0</v>
       </c>
+      <c r="IX86">
+        <v>0</v>
+      </c>
     </row>
-    <row r="87" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>287</v>
       </c>
@@ -65838,8 +66099,11 @@
       <c r="IW87">
         <v>0</v>
       </c>
+      <c r="IX87">
+        <v>0</v>
+      </c>
     </row>
-    <row r="88" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>292</v>
       </c>
@@ -66593,8 +66857,11 @@
       <c r="IW88">
         <v>0</v>
       </c>
+      <c r="IX88">
+        <v>5</v>
+      </c>
     </row>
-    <row r="89" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>294</v>
       </c>
@@ -67336,8 +67603,11 @@
       <c r="IW89">
         <v>0</v>
       </c>
+      <c r="IX89">
+        <v>0</v>
+      </c>
     </row>
-    <row r="90" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>306</v>
       </c>
@@ -68088,8 +68358,11 @@
       <c r="IW90">
         <v>0</v>
       </c>
+      <c r="IX90">
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>255</v>
       </c>
@@ -68813,8 +69086,11 @@
       <c r="IW91">
         <v>0</v>
       </c>
+      <c r="IX91">
+        <v>0</v>
+      </c>
     </row>
-    <row r="92" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>257</v>
       </c>
@@ -69535,8 +69811,11 @@
       <c r="IW92">
         <v>0</v>
       </c>
+      <c r="IX92">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>260</v>
       </c>
@@ -70272,8 +70551,11 @@
       <c r="IW93">
         <v>0</v>
       </c>
+      <c r="IX93">
+        <v>0</v>
+      </c>
     </row>
-    <row r="94" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>264</v>
       </c>
@@ -70997,8 +71279,11 @@
       <c r="IW94">
         <v>0</v>
       </c>
+      <c r="IX94">
+        <v>0</v>
+      </c>
     </row>
-    <row r="95" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>265</v>
       </c>
@@ -71722,8 +72007,11 @@
       <c r="IW95">
         <v>0</v>
       </c>
+      <c r="IX95">
+        <v>0</v>
+      </c>
     </row>
-    <row r="96" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>266</v>
       </c>
@@ -72444,8 +72732,11 @@
       <c r="IW96">
         <v>0</v>
       </c>
+      <c r="IX96">
+        <v>0</v>
+      </c>
     </row>
-    <row r="97" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>268</v>
       </c>
@@ -73175,8 +73466,11 @@
       <c r="IW97">
         <v>0</v>
       </c>
+      <c r="IX97">
+        <v>0</v>
+      </c>
     </row>
-    <row r="98" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>270</v>
       </c>
@@ -73906,8 +74200,11 @@
       <c r="IW98">
         <v>0</v>
       </c>
+      <c r="IX98">
+        <v>0</v>
+      </c>
     </row>
-    <row r="99" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>271</v>
       </c>
@@ -74625,8 +74922,11 @@
       <c r="IW99">
         <v>0</v>
       </c>
+      <c r="IX99">
+        <v>0</v>
+      </c>
     </row>
-    <row r="100" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>272</v>
       </c>
@@ -75353,8 +75653,11 @@
       <c r="IW100">
         <v>0</v>
       </c>
+      <c r="IX100">
+        <v>0</v>
+      </c>
     </row>
-    <row r="101" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>276</v>
       </c>
@@ -76069,8 +76372,11 @@
       <c r="IW101">
         <v>0</v>
       </c>
+      <c r="IX101">
+        <v>0</v>
+      </c>
     </row>
-    <row r="102" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>280</v>
       </c>
@@ -76788,8 +77094,11 @@
       <c r="IW102">
         <v>0</v>
       </c>
+      <c r="IX102">
+        <v>0</v>
+      </c>
     </row>
-    <row r="103" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>281</v>
       </c>
@@ -77504,8 +77813,11 @@
       <c r="IW103">
         <v>0</v>
       </c>
+      <c r="IX103">
+        <v>0</v>
+      </c>
     </row>
-    <row r="104" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>282</v>
       </c>
@@ -78232,8 +78544,11 @@
       <c r="IW104">
         <v>0</v>
       </c>
+      <c r="IX104">
+        <v>0</v>
+      </c>
     </row>
-    <row r="105" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>283</v>
       </c>
@@ -78966,8 +79281,11 @@
       <c r="IW105">
         <v>0</v>
       </c>
+      <c r="IX105">
+        <v>0</v>
+      </c>
     </row>
-    <row r="106" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>285</v>
       </c>
@@ -79715,8 +80033,11 @@
       <c r="IW106">
         <v>0</v>
       </c>
+      <c r="IX106">
+        <v>1</v>
+      </c>
     </row>
-    <row r="107" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>287</v>
       </c>
@@ -80449,8 +80770,11 @@
       <c r="IW107">
         <v>0</v>
       </c>
+      <c r="IX107">
+        <v>0</v>
+      </c>
     </row>
-    <row r="108" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>288</v>
       </c>
@@ -81189,8 +81513,11 @@
       <c r="IW108">
         <v>0</v>
       </c>
+      <c r="IX108">
+        <v>0</v>
+      </c>
     </row>
-    <row r="109" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>291</v>
       </c>
@@ -81887,8 +82214,11 @@
       <c r="IW109">
         <v>0</v>
       </c>
+      <c r="IX109">
+        <v>0</v>
+      </c>
     </row>
-    <row r="110" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>292</v>
       </c>
@@ -82615,8 +82945,11 @@
       <c r="IW110">
         <v>0</v>
       </c>
+      <c r="IX110">
+        <v>0</v>
+      </c>
     </row>
-    <row r="111" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>293</v>
       </c>
@@ -83349,8 +83682,11 @@
       <c r="IW111">
         <v>0</v>
       </c>
+      <c r="IX111">
+        <v>1</v>
+      </c>
     </row>
-    <row r="112" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>294</v>
       </c>
@@ -84083,8 +84419,11 @@
       <c r="IW112">
         <v>0</v>
       </c>
+      <c r="IX112">
+        <v>1</v>
+      </c>
     </row>
-    <row r="113" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>297</v>
       </c>
@@ -84811,8 +85150,11 @@
       <c r="IW113">
         <v>0</v>
       </c>
+      <c r="IX113">
+        <v>0</v>
+      </c>
     </row>
-    <row r="114" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>299</v>
       </c>
@@ -85542,8 +85884,11 @@
       <c r="IW114">
         <v>0</v>
       </c>
+      <c r="IX114">
+        <v>0</v>
+      </c>
     </row>
-    <row r="115" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>301</v>
       </c>
@@ -86273,8 +86618,11 @@
       <c r="IW115">
         <v>0</v>
       </c>
+      <c r="IX115">
+        <v>0</v>
+      </c>
     </row>
-    <row r="116" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>303</v>
       </c>
@@ -86971,8 +87319,11 @@
       <c r="IW116">
         <v>0</v>
       </c>
+      <c r="IX116">
+        <v>0</v>
+      </c>
     </row>
-    <row r="117" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>305</v>
       </c>
@@ -87702,8 +88053,11 @@
       <c r="IW117">
         <v>0</v>
       </c>
+      <c r="IX117">
+        <v>0</v>
+      </c>
     </row>
-    <row r="118" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>306</v>
       </c>
@@ -88424,8 +88778,11 @@
       <c r="IW118">
         <v>0</v>
       </c>
+      <c r="IX118">
+        <v>0</v>
+      </c>
     </row>
-    <row r="119" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>308</v>
       </c>
@@ -89149,8 +89506,11 @@
       <c r="IW119">
         <v>0</v>
       </c>
+      <c r="IX119">
+        <v>0</v>
+      </c>
     </row>
-    <row r="120" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>309</v>
       </c>
@@ -89877,8 +90237,11 @@
       <c r="IW120">
         <v>0</v>
       </c>
+      <c r="IX120">
+        <v>0</v>
+      </c>
     </row>
-    <row r="121" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>310</v>
       </c>
@@ -90596,8 +90959,11 @@
       <c r="IW121">
         <v>0</v>
       </c>
+      <c r="IX121">
+        <v>0</v>
+      </c>
     </row>
-    <row r="122" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>311</v>
       </c>
@@ -91348,8 +91714,11 @@
       <c r="IW122">
         <v>0</v>
       </c>
+      <c r="IX122">
+        <v>1</v>
+      </c>
     </row>
-    <row r="123" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>229</v>
       </c>
@@ -92094,8 +92463,11 @@
       <c r="IW123">
         <v>0</v>
       </c>
+      <c r="IX123">
+        <v>0</v>
+      </c>
     </row>
-    <row r="124" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>314</v>
       </c>
@@ -92843,8 +93215,11 @@
       <c r="IW124">
         <v>0</v>
       </c>
+      <c r="IX124">
+        <v>1</v>
+      </c>
     </row>
-    <row r="125" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>316</v>
       </c>
@@ -93571,8 +93946,11 @@
       <c r="IW125">
         <v>0</v>
       </c>
+      <c r="IX125">
+        <v>0</v>
+      </c>
     </row>
-    <row r="126" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>317</v>
       </c>
@@ -94302,8 +94680,11 @@
       <c r="IW126">
         <v>0</v>
       </c>
+      <c r="IX126">
+        <v>0</v>
+      </c>
     </row>
-    <row r="127" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>319</v>
       </c>
@@ -95039,8 +95420,11 @@
       <c r="IW127">
         <v>0</v>
       </c>
+      <c r="IX127">
+        <v>0</v>
+      </c>
     </row>
-    <row r="128" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>320</v>
       </c>
@@ -95788,8 +96172,11 @@
       <c r="IW128">
         <v>0</v>
       </c>
+      <c r="IX128">
+        <v>15</v>
+      </c>
     </row>
-    <row r="129" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>321</v>
       </c>
@@ -96522,8 +96909,11 @@
       <c r="IW129">
         <v>0</v>
       </c>
+      <c r="IX129">
+        <v>0</v>
+      </c>
     </row>
-    <row r="130" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>322</v>
       </c>
@@ -97256,8 +97646,11 @@
       <c r="IW130">
         <v>0</v>
       </c>
+      <c r="IX130">
+        <v>0</v>
+      </c>
     </row>
-    <row r="131" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>323</v>
       </c>
@@ -97972,8 +98365,11 @@
       <c r="IW131">
         <v>0</v>
       </c>
+      <c r="IX131">
+        <v>0</v>
+      </c>
     </row>
-    <row r="132" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>324</v>
       </c>
@@ -98721,8 +99117,11 @@
       <c r="IW132">
         <v>0</v>
       </c>
+      <c r="IX132">
+        <v>0</v>
+      </c>
     </row>
-    <row r="133" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>325</v>
       </c>
@@ -99443,8 +99842,11 @@
       <c r="IW133">
         <v>0</v>
       </c>
+      <c r="IX133">
+        <v>0</v>
+      </c>
     </row>
-    <row r="134" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>327</v>
       </c>
@@ -100174,8 +100576,11 @@
       <c r="IW134">
         <v>0</v>
       </c>
+      <c r="IX134">
+        <v>4</v>
+      </c>
     </row>
-    <row r="135" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>329</v>
       </c>
@@ -100917,8 +101322,11 @@
       <c r="IW135">
         <v>0</v>
       </c>
+      <c r="IX135">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>330</v>
       </c>
@@ -101651,8 +102059,11 @@
       <c r="IW136">
         <v>0</v>
       </c>
+      <c r="IX136">
+        <v>0</v>
+      </c>
     </row>
-    <row r="137" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>332</v>
       </c>
@@ -102397,8 +102808,11 @@
       <c r="IW137">
         <v>0</v>
       </c>
+      <c r="IX137">
+        <v>0</v>
+      </c>
     </row>
-    <row r="138" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>333</v>
       </c>
@@ -103131,8 +103545,11 @@
       <c r="IW138">
         <v>0</v>
       </c>
+      <c r="IX138">
+        <v>0</v>
+      </c>
     </row>
-    <row r="139" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>334</v>
       </c>
@@ -103886,8 +104303,11 @@
       <c r="IW139">
         <v>0</v>
       </c>
+      <c r="IX139">
+        <v>0</v>
+      </c>
     </row>
-    <row r="140" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>336</v>
       </c>
@@ -104629,8 +105049,11 @@
       <c r="IW140">
         <v>0</v>
       </c>
+      <c r="IX140">
+        <v>0</v>
+      </c>
     </row>
-    <row r="141" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>221</v>
       </c>
@@ -105378,8 +105801,11 @@
       <c r="IW141">
         <v>0</v>
       </c>
+      <c r="IX141">
+        <v>1</v>
+      </c>
     </row>
-    <row r="142" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>337</v>
       </c>
@@ -106109,8 +106535,11 @@
       <c r="IW142">
         <v>0</v>
       </c>
+      <c r="IX142">
+        <v>0</v>
+      </c>
     </row>
-    <row r="143" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>220</v>
       </c>
@@ -106846,8 +107275,11 @@
       <c r="IW143">
         <v>0</v>
       </c>
+      <c r="IX143">
+        <v>42</v>
+      </c>
     </row>
-    <row r="144" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>338</v>
       </c>
@@ -107568,8 +108000,11 @@
       <c r="IW144">
         <v>0</v>
       </c>
+      <c r="IX144">
+        <v>2</v>
+      </c>
     </row>
-    <row r="145" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>339</v>
       </c>
@@ -108326,8 +108761,11 @@
       <c r="IW145">
         <v>0</v>
       </c>
+      <c r="IX145">
+        <v>1</v>
+      </c>
     </row>
-    <row r="146" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>341</v>
       </c>
@@ -109063,8 +109501,11 @@
       <c r="IW146">
         <v>0</v>
       </c>
+      <c r="IX146">
+        <v>0</v>
+      </c>
     </row>
-    <row r="147" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>342</v>
       </c>
@@ -109788,8 +110229,11 @@
       <c r="IW147">
         <v>0</v>
       </c>
+      <c r="IX147">
+        <v>0</v>
+      </c>
     </row>
-    <row r="148" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>343</v>
       </c>
@@ -110516,8 +110960,11 @@
       <c r="IW148">
         <v>0</v>
       </c>
+      <c r="IX148">
+        <v>0</v>
+      </c>
     </row>
-    <row r="149" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>344</v>
       </c>
@@ -111259,8 +111706,11 @@
       <c r="IW149">
         <v>0</v>
       </c>
+      <c r="IX149">
+        <v>1</v>
+      </c>
     </row>
-    <row r="150" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>345</v>
       </c>
@@ -112008,8 +112458,11 @@
       <c r="IW150">
         <v>0</v>
       </c>
+      <c r="IX150">
+        <v>0</v>
+      </c>
     </row>
-    <row r="151" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>346</v>
       </c>
@@ -112754,8 +113207,11 @@
       <c r="IW151">
         <v>0</v>
       </c>
+      <c r="IX151">
+        <v>0</v>
+      </c>
     </row>
-    <row r="152" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>347</v>
       </c>
@@ -113482,8 +113938,11 @@
       <c r="IW152">
         <v>0</v>
       </c>
+      <c r="IX152">
+        <v>0</v>
+      </c>
     </row>
-    <row r="153" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>348</v>
       </c>
@@ -114204,8 +114663,11 @@
       <c r="IW153">
         <v>0</v>
       </c>
+      <c r="IX153">
+        <v>0</v>
+      </c>
     </row>
-    <row r="154" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>349</v>
       </c>
@@ -114926,8 +115388,11 @@
       <c r="IW154">
         <v>0</v>
       </c>
+      <c r="IX154">
+        <v>0</v>
+      </c>
     </row>
-    <row r="155" spans="1:257" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:258" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>350</v>
       </c>
@@ -115625,6 +116090,9 @@
         <v>0</v>
       </c>
       <c r="IW155">
+        <v>0</v>
+      </c>
+      <c r="IX155">
         <v>0</v>
       </c>
     </row>

</xml_diff>